<commit_message>
results de mlp no texto
</commit_message>
<xml_diff>
--- a/T4/MLP.xlsx
+++ b/T4/MLP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>MULTILAYER PERCEPTRON</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>Total Insts</t>
+  </si>
+  <si>
+    <t>Para N = 100 e L = 0.5</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Precisao</t>
+  </si>
+  <si>
+    <t>Abrangencia</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Media:</t>
   </si>
 </sst>
 </file>
@@ -159,11 +177,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -176,11 +191,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -466,11 +524,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="421263656"/>
-        <c:axId val="421261304"/>
+        <c:axId val="421302064"/>
+        <c:axId val="421302456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="421263656"/>
+        <c:axId val="421302064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +568,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421261304"/>
+        <c:crossAx val="421302456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -518,7 +576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421261304"/>
+        <c:axId val="421302456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,7 +674,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="421263656"/>
+        <c:crossAx val="421302064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1274,6 +1332,18 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A30:D41" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <tableColumns count="4">
+    <tableColumn id="1" name="Classe" dataDxfId="5"/>
+    <tableColumn id="2" name="Precisao" dataDxfId="4"/>
+    <tableColumn id="3" name="Abrangencia" dataDxfId="3"/>
+    <tableColumn id="4" name="F1" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1539,619 +1609,794 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1725</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>72</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.95550000000000002</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>1.5100000000000001E-2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>8.0199999999999994E-2</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>8.3625000000000007</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>26.721800000000002</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>50</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>1738</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>59</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.96350000000000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>5.4320000000000004</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>23.868300000000001</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>100</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>1742</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>55</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.96599999999999997</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>7.0400000000000004E-2</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>4.9076000000000004</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>23.476900000000001</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>250</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>1741</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>56</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>0.96540000000000004</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>8.3000000000000001E-3</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>4.6216999999999997</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>23.655999999999999</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>500</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>1741</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>56</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>0.96540000000000004</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>8.0999999999999996E-3</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>7.17E-2</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>4.5262000000000002</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>23.9129</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>750</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>1740</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>57</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>0.96479999999999999</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>7.17E-2</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>4.4248000000000003</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>23.887799999999999</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>1000</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>1740</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>57</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>0.96479999999999999</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>7.17E-2</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>4.3704999999999998</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>23.9009</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>5000</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>1741</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>56</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0.96540000000000004</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>4.1435000000000004</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>23.999700000000001</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>10000</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>1741</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>56</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>0.96540000000000004</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>7.2099999999999997E-2</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>4.0701000000000001</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>24.029199999999999</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>10</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>1715</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>82</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>0.94930000000000003</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>8.3900000000000002E-2</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>9.6913</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>27.965599999999998</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>50</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>1734</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>63</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>0.96099999999999997</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>1.11E-2</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <v>6.1555</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>24.989899999999999</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>100</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>1737</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>60</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>0.96289999999999998</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>1.04E-2</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>7.4899999999999994E-2</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>5.7671999999999999</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>24.9602</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>250</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1733</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>64</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>0.96040000000000003</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>7.6600000000000001E-2</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>5.4642999999999997</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>25.549600000000002</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>500</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>1735</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>62</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>0.9617</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>5.2107999999999999</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>25.590199999999999</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>750</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>1735</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>62</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>0.9617</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>5.1139000000000001</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>25.648800000000001</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>1000</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>1735</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>62</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>0.9617</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>7.7100000000000002E-2</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>5.0613000000000001</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>25.706600000000002</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>5000</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>1729</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>68</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>0.95799999999999996</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>7.8899999999999998E-2</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>4.9512</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>26.310500000000001</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="2">
         <v>1797</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>10000</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>1730</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>67</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>0.95860000000000001</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>7.9299999999999995E-2</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>4.9004000000000003</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>26.443999999999999</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="2">
         <v>1797</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>0</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.99199999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>1</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.995</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.97099999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>2</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.98599999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>3</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>4</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>5</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>6</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>7</v>
+      </c>
+      <c r="B38" s="6">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.95099999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>8</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>9</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.94599999999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="6">
+        <v>0.97</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.96899999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -2161,5 +2406,8 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>